<commit_message>
Administracion del sprint 1 actualizado
Terminado el archivo de administración del sprint 1
</commit_message>
<xml_diff>
--- a/Admistracion grupal sprint 1.xlsx
+++ b/Admistracion grupal sprint 1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="SPRINT 0 ACTIVIDADES" sheetId="1" r:id="rId1"/>
@@ -29,10 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="37">
-  <si>
-    <t>ACTIVIDADES SPRINT 0</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="61">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -130,16 +127,91 @@
     <t>TOTAL SPRINT</t>
   </si>
   <si>
-    <t>Rediseño de diagramas</t>
-  </si>
-  <si>
-    <t>Implementacion de recursos</t>
-  </si>
-  <si>
     <t>Reuniones grupales</t>
   </si>
   <si>
     <t>SPRINT 1</t>
+  </si>
+  <si>
+    <t>Instalacion de programas</t>
+  </si>
+  <si>
+    <t>Reunion grupal</t>
+  </si>
+  <si>
+    <t>Reunion con Taller IV</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Documentacion de sprint 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reinstalacion programas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testeo y pruebas HTML </t>
+  </si>
+  <si>
+    <t>Reunion Grupal</t>
+  </si>
+  <si>
+    <t>Reunion Taller IV</t>
+  </si>
+  <si>
+    <t>Implementacion primeras caract de editor</t>
+  </si>
+  <si>
+    <t>Elaboracion presentacion sprint 1</t>
+  </si>
+  <si>
+    <t>Pruebas de futuros componentes</t>
+  </si>
+  <si>
+    <t>Reunion con taller IV</t>
+  </si>
+  <si>
+    <t>Rediseño de diagrama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pruebas con menus desplegables </t>
+  </si>
+  <si>
+    <t>Implementacion menus en beta</t>
+  </si>
+  <si>
+    <t>Estudio de nuevos complementos</t>
+  </si>
+  <si>
+    <t>Estudio presentacion sprint</t>
+  </si>
+  <si>
+    <t>Testeos de login definitivo</t>
+  </si>
+  <si>
+    <t>Prueba login y index</t>
+  </si>
+  <si>
+    <t>Implementacion login beta</t>
+  </si>
+  <si>
+    <t>ACTIVIDADES SPRINT 1</t>
+  </si>
+  <si>
+    <t>Testeo de recursos</t>
+  </si>
+  <si>
+    <t>Desarrollo de primeros recursos</t>
+  </si>
+  <si>
+    <t>Implementacion en beta version 1.0</t>
+  </si>
+  <si>
+    <t>Documentaciones</t>
+  </si>
+  <si>
+    <t>Pruebas futuros comp</t>
   </si>
 </sst>
 </file>
@@ -366,7 +438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -377,6 +449,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -385,44 +464,36 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,6 +587,18 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -791,6 +874,18 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1066,6 +1161,18 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1341,6 +1448,18 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1607,6 +1726,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2168,8 +2296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G1:M1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2178,8 +2306,8 @@
     <col min="6" max="6" width="8.09765625" customWidth="1"/>
     <col min="7" max="8" width="9.3984375" customWidth="1"/>
     <col min="9" max="9" width="12.5" customWidth="1"/>
-    <col min="10" max="10" width="16.3984375" customWidth="1"/>
-    <col min="11" max="11" width="15.59765625" customWidth="1"/>
+    <col min="10" max="10" width="16.796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.09765625" bestFit="1" customWidth="1"/>
     <col min="12" max="15" width="9.3984375" customWidth="1"/>
     <col min="16" max="16" width="12.69921875" customWidth="1"/>
     <col min="17" max="26" width="9.3984375" customWidth="1"/>
@@ -2187,20 +2315,20 @@
   <sheetData>
     <row r="1" spans="7:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="7:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G2" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
+      <c r="G2" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
     </row>
     <row r="3" spans="7:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
     </row>
     <row r="4" spans="7:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="G4" s="1"/>
@@ -2211,175 +2339,211 @@
     </row>
     <row r="5" spans="7:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G5" s="19" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="20"/>
       <c r="I5" s="21"/>
       <c r="J5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="2" t="s">
+    </row>
+    <row r="6" spans="7:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="7:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="23">
+        <v>8</v>
+      </c>
+      <c r="K6" s="23">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="7:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G7" s="11"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="M7" s="27"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="M7" s="8"/>
     </row>
     <row r="8" spans="7:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="12"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="23">
+        <v>8</v>
+      </c>
+      <c r="K8" s="23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="7:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="14"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+    </row>
+    <row r="10" spans="7:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="12"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="23">
+        <v>12</v>
+      </c>
+      <c r="K10" s="23">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="7:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="14"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+    </row>
+    <row r="12" spans="7:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="12"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="23">
+        <v>8</v>
+      </c>
+      <c r="K12" s="23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="7:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="14"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+    </row>
+    <row r="14" spans="7:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" s="12"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="23">
+        <v>8</v>
+      </c>
+      <c r="K14" s="23"/>
+    </row>
+    <row r="15" spans="7:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G15" s="14"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+    </row>
+    <row r="16" spans="7:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G16" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" s="12"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23">
+        <v>6</v>
+      </c>
+      <c r="L16" s="9"/>
+    </row>
+    <row r="17" spans="7:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="14"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="10"/>
+    </row>
+    <row r="18" spans="7:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G18" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18" s="12"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="23">
+        <v>8</v>
+      </c>
+      <c r="K18" s="23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="7:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="14"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+    </row>
+    <row r="20" spans="7:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="11"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+    </row>
+    <row r="21" spans="7:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G21" s="14"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+    </row>
+    <row r="22" spans="7:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G22" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" s="12"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="23">
         <v>4</v>
       </c>
-      <c r="H8" s="9"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-    </row>
-    <row r="9" spans="7:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G9" s="11"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-    </row>
-    <row r="10" spans="7:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G10" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-    </row>
-    <row r="11" spans="7:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G11" s="11"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-    </row>
-    <row r="12" spans="7:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G12" s="8"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-    </row>
-    <row r="13" spans="7:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G13" s="11"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-    </row>
-    <row r="14" spans="7:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G14" s="8"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-    </row>
-    <row r="15" spans="7:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G15" s="11"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-    </row>
-    <row r="16" spans="7:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G16" s="8"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="28"/>
-    </row>
-    <row r="17" spans="7:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G17" s="11"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="29"/>
-    </row>
-    <row r="18" spans="7:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G18" s="8"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-    </row>
-    <row r="19" spans="7:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G19" s="11"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-    </row>
-    <row r="20" spans="7:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G20" s="8"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
-    </row>
-    <row r="21" spans="7:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G21" s="11"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-    </row>
-    <row r="22" spans="7:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G22" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H22" s="9"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
+      <c r="K22" s="23">
+        <v>4</v>
+      </c>
     </row>
     <row r="23" spans="7:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G23" s="11"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
     </row>
     <row r="24" spans="7:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G24" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="H24" s="9"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="16">
+      <c r="G24" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" s="12"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="23">
         <f t="shared" ref="J24:K24" si="0">J22+J20+J18+J16+J14+J12+J10+J6</f>
-        <v>0</v>
-      </c>
-      <c r="K24" s="16">
+        <v>48</v>
+      </c>
+      <c r="K24" s="23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="7:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G25" s="11"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="28"/>
     </row>
     <row r="26" spans="7:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="7:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3358,23 +3522,6 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="G10:I11"/>
-    <mergeCell ref="G12:I13"/>
-    <mergeCell ref="G2:K3"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="G8:I9"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="G6:I7"/>
     <mergeCell ref="G14:I15"/>
     <mergeCell ref="G16:I17"/>
     <mergeCell ref="G24:I25"/>
@@ -3390,6 +3537,23 @@
     <mergeCell ref="G20:I21"/>
     <mergeCell ref="K14:K15"/>
     <mergeCell ref="J14:J15"/>
+    <mergeCell ref="G10:I11"/>
+    <mergeCell ref="G12:I13"/>
+    <mergeCell ref="G2:K3"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="G8:I9"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="G6:I7"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -3400,37 +3564,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="9.3984375" customWidth="1"/>
-    <col min="4" max="4" width="12.8984375" customWidth="1"/>
+    <col min="4" max="4" width="13.09765625" customWidth="1"/>
     <col min="5" max="26" width="9.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G1" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
+        <v>33</v>
+      </c>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
     </row>
     <row r="2" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
     </row>
     <row r="3" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
@@ -3439,7 +3603,7 @@
       <c r="G4" s="20"/>
       <c r="H4" s="21"/>
       <c r="J4" s="19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K4" s="20"/>
       <c r="L4" s="20"/>
@@ -3450,10 +3614,10 @@
     </row>
     <row r="5" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="24" t="s">
         <v>8</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>9</v>
       </c>
       <c r="D5" s="20"/>
       <c r="E5" s="20"/>
@@ -3461,10 +3625,10 @@
       <c r="G5" s="20"/>
       <c r="H5" s="21"/>
       <c r="J5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="24" t="s">
         <v>8</v>
-      </c>
-      <c r="K5" s="23" t="s">
-        <v>9</v>
       </c>
       <c r="L5" s="20"/>
       <c r="M5" s="20"/>
@@ -3473,149 +3637,209 @@
       <c r="P5" s="21"/>
     </row>
     <row r="6" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="24" t="s">
-        <v>1</v>
+      <c r="B6" s="26" t="s">
+        <v>0</v>
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="21"/>
       <c r="E6" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H6" s="21"/>
-      <c r="J6" s="24" t="s">
-        <v>1</v>
+      <c r="J6" s="26" t="s">
+        <v>0</v>
       </c>
       <c r="K6" s="20"/>
       <c r="L6" s="21"/>
       <c r="M6" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N6" s="21"/>
       <c r="O6" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P6" s="21"/>
     </row>
     <row r="7" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="23"/>
+      <c r="B7" s="24" t="s">
+        <v>3</v>
+      </c>
       <c r="C7" s="20"/>
       <c r="D7" s="21"/>
-      <c r="E7" s="23"/>
+      <c r="E7" s="24">
+        <v>2</v>
+      </c>
       <c r="F7" s="21"/>
-      <c r="G7" s="23"/>
+      <c r="G7" s="24">
+        <v>2</v>
+      </c>
       <c r="H7" s="21"/>
-      <c r="J7" s="23"/>
+      <c r="J7" s="24" t="s">
+        <v>39</v>
+      </c>
       <c r="K7" s="20"/>
       <c r="L7" s="21"/>
-      <c r="M7" s="23"/>
+      <c r="M7" s="24">
+        <v>1</v>
+      </c>
       <c r="N7" s="21"/>
-      <c r="O7" s="23"/>
+      <c r="O7" s="24">
+        <v>1</v>
+      </c>
       <c r="P7" s="21"/>
     </row>
     <row r="8" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="23"/>
+      <c r="B8" s="24" t="s">
+        <v>34</v>
+      </c>
       <c r="C8" s="20"/>
       <c r="D8" s="21"/>
-      <c r="E8" s="23"/>
+      <c r="E8" s="24">
+        <v>2</v>
+      </c>
       <c r="F8" s="21"/>
-      <c r="G8" s="23"/>
+      <c r="G8" s="24">
+        <v>2</v>
+      </c>
       <c r="H8" s="21"/>
-      <c r="J8" s="23"/>
+      <c r="J8" s="24" t="s">
+        <v>40</v>
+      </c>
       <c r="K8" s="20"/>
       <c r="L8" s="21"/>
-      <c r="M8" s="23"/>
+      <c r="M8" s="24">
+        <v>3</v>
+      </c>
       <c r="N8" s="21"/>
-      <c r="O8" s="23"/>
+      <c r="O8" s="24">
+        <v>3</v>
+      </c>
       <c r="P8" s="21"/>
     </row>
     <row r="9" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="23"/>
+      <c r="B9" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="C9" s="20"/>
       <c r="D9" s="21"/>
-      <c r="E9" s="19"/>
+      <c r="E9" s="24">
+        <v>1</v>
+      </c>
       <c r="F9" s="21"/>
-      <c r="G9" s="23"/>
+      <c r="G9" s="24">
+        <v>1</v>
+      </c>
       <c r="H9" s="21"/>
-      <c r="J9" s="23"/>
+      <c r="J9" s="24" t="s">
+        <v>41</v>
+      </c>
       <c r="K9" s="20"/>
       <c r="L9" s="21"/>
-      <c r="M9" s="19"/>
+      <c r="M9" s="24">
+        <v>1</v>
+      </c>
       <c r="N9" s="21"/>
-      <c r="O9" s="23"/>
+      <c r="O9" s="24">
+        <v>1</v>
+      </c>
       <c r="P9" s="21"/>
     </row>
     <row r="10" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="23"/>
+      <c r="B10" s="24" t="s">
+        <v>36</v>
+      </c>
       <c r="C10" s="20"/>
       <c r="D10" s="21"/>
-      <c r="E10" s="23"/>
+      <c r="E10" s="24" t="s">
+        <v>37</v>
+      </c>
       <c r="F10" s="21"/>
-      <c r="G10" s="23"/>
+      <c r="G10" s="24">
+        <v>2</v>
+      </c>
       <c r="H10" s="21"/>
-      <c r="J10" s="23"/>
+      <c r="J10" s="24" t="s">
+        <v>42</v>
+      </c>
       <c r="K10" s="20"/>
       <c r="L10" s="21"/>
-      <c r="M10" s="23"/>
+      <c r="M10" s="24" t="s">
+        <v>37</v>
+      </c>
       <c r="N10" s="21"/>
-      <c r="O10" s="23"/>
+      <c r="O10" s="24">
+        <v>1</v>
+      </c>
       <c r="P10" s="21"/>
     </row>
     <row r="11" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="23"/>
+      <c r="B11" s="24" t="s">
+        <v>38</v>
+      </c>
       <c r="C11" s="20"/>
       <c r="D11" s="21"/>
-      <c r="E11" s="23"/>
+      <c r="E11" s="24" t="s">
+        <v>37</v>
+      </c>
       <c r="F11" s="21"/>
-      <c r="G11" s="23"/>
+      <c r="G11" s="24">
+        <v>1</v>
+      </c>
       <c r="H11" s="21"/>
-      <c r="J11" s="23"/>
+      <c r="J11" s="24" t="s">
+        <v>38</v>
+      </c>
       <c r="K11" s="20"/>
       <c r="L11" s="21"/>
-      <c r="M11" s="23"/>
+      <c r="M11" s="24" t="s">
+        <v>37</v>
+      </c>
       <c r="N11" s="21"/>
-      <c r="O11" s="23"/>
+      <c r="O11" s="24">
+        <v>1</v>
+      </c>
       <c r="P11" s="21"/>
     </row>
     <row r="12" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="21"/>
       <c r="E12" s="19">
         <f>SUM(E7:F11)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="19">
         <f>SUM(G7:H11)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H12" s="21"/>
       <c r="J12" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K12" s="20"/>
       <c r="L12" s="21"/>
       <c r="M12" s="19">
         <f>SUM(M7:N11)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N12" s="21"/>
       <c r="O12" s="19">
         <f>SUM(O7:P11)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="P12" s="21"/>
     </row>
     <row r="13" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
@@ -3624,7 +3848,7 @@
       <c r="G14" s="20"/>
       <c r="H14" s="21"/>
       <c r="J14" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K14" s="20"/>
       <c r="L14" s="20"/>
@@ -3634,10 +3858,10 @@
     </row>
     <row r="15" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="24" t="s">
         <v>8</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>9</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="20"/>
@@ -3646,54 +3870,71 @@
       <c r="H15" s="21"/>
       <c r="J15" s="4"/>
       <c r="K15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="M15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="N15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N15" s="2" t="s">
+      <c r="O15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O15" s="3" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="16" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="24" t="s">
-        <v>1</v>
+      <c r="B16" s="26" t="s">
+        <v>0</v>
       </c>
       <c r="C16" s="20"/>
       <c r="D16" s="21"/>
       <c r="E16" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H16" s="21"/>
       <c r="J16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="K16" s="4">
+        <v>15</v>
+      </c>
+      <c r="L16" s="4">
+        <f>K17-G12</f>
+        <v>7</v>
+      </c>
+      <c r="M16" s="4">
+        <v>0</v>
+      </c>
+      <c r="N16" s="4">
+        <v>0</v>
+      </c>
+      <c r="O16" s="4">
+        <v>9</v>
+      </c>
     </row>
     <row r="17" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="23"/>
+      <c r="B17" s="24" t="s">
+        <v>43</v>
+      </c>
       <c r="C17" s="20"/>
       <c r="D17" s="21"/>
-      <c r="E17" s="23"/>
+      <c r="E17" s="24">
+        <v>2</v>
+      </c>
       <c r="F17" s="21"/>
-      <c r="G17" s="23"/>
+      <c r="G17" s="24">
+        <v>3</v>
+      </c>
       <c r="H17" s="21"/>
       <c r="J17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K17" s="4">
         <v>15</v>
@@ -3712,82 +3953,112 @@
       </c>
     </row>
     <row r="18" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="23"/>
+      <c r="B18" s="24" t="s">
+        <v>45</v>
+      </c>
       <c r="C18" s="20"/>
       <c r="D18" s="21"/>
-      <c r="E18" s="23"/>
+      <c r="E18" s="24">
+        <v>2</v>
+      </c>
       <c r="F18" s="21"/>
-      <c r="G18" s="23"/>
+      <c r="G18" s="24">
+        <v>2</v>
+      </c>
       <c r="H18" s="21"/>
     </row>
     <row r="19" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="23"/>
+      <c r="B19" s="24" t="s">
+        <v>41</v>
+      </c>
       <c r="C19" s="20"/>
       <c r="D19" s="21"/>
-      <c r="E19" s="19"/>
+      <c r="E19" s="24">
+        <v>1</v>
+      </c>
       <c r="F19" s="21"/>
-      <c r="G19" s="23"/>
+      <c r="G19" s="24">
+        <v>1</v>
+      </c>
       <c r="H19" s="21"/>
     </row>
     <row r="20" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="23"/>
+      <c r="B20" s="24" t="s">
+        <v>46</v>
+      </c>
       <c r="C20" s="20"/>
       <c r="D20" s="21"/>
-      <c r="E20" s="23"/>
+      <c r="E20" s="24" t="s">
+        <v>37</v>
+      </c>
       <c r="F20" s="21"/>
-      <c r="G20" s="23"/>
+      <c r="G20" s="24">
+        <v>1</v>
+      </c>
       <c r="H20" s="21"/>
     </row>
     <row r="21" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="23"/>
+      <c r="B21" s="24" t="s">
+        <v>38</v>
+      </c>
       <c r="C21" s="20"/>
       <c r="D21" s="21"/>
-      <c r="E21" s="23"/>
+      <c r="E21" s="24" t="s">
+        <v>37</v>
+      </c>
       <c r="F21" s="21"/>
-      <c r="G21" s="23"/>
+      <c r="G21" s="24">
+        <v>1</v>
+      </c>
       <c r="H21" s="21"/>
     </row>
     <row r="22" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="23"/>
+      <c r="B22" s="24" t="s">
+        <v>44</v>
+      </c>
       <c r="C22" s="20"/>
       <c r="D22" s="21"/>
-      <c r="E22" s="23"/>
+      <c r="E22" s="24" t="s">
+        <v>37</v>
+      </c>
       <c r="F22" s="21"/>
-      <c r="G22" s="23"/>
+      <c r="G22" s="24">
+        <v>1</v>
+      </c>
       <c r="H22" s="21"/>
     </row>
     <row r="23" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="23"/>
+      <c r="B23" s="24"/>
       <c r="C23" s="20"/>
       <c r="D23" s="21"/>
-      <c r="E23" s="23"/>
+      <c r="E23" s="24"/>
       <c r="F23" s="21"/>
-      <c r="G23" s="23"/>
+      <c r="G23" s="24"/>
       <c r="H23" s="21"/>
     </row>
     <row r="24" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="23"/>
+      <c r="B24" s="24"/>
       <c r="C24" s="20"/>
       <c r="D24" s="21"/>
-      <c r="E24" s="23"/>
+      <c r="E24" s="24"/>
       <c r="F24" s="21"/>
-      <c r="G24" s="23"/>
+      <c r="G24" s="24"/>
       <c r="H24" s="21"/>
     </row>
     <row r="25" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C25" s="20"/>
       <c r="D25" s="21"/>
       <c r="E25" s="19">
         <f>SUM(E17:F24)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F25" s="21"/>
       <c r="G25" s="19">
         <f>SUM(G17:H24)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H25" s="21"/>
     </row>
@@ -4768,21 +5039,52 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="J14:O14"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="J4:P4"/>
+    <mergeCell ref="K5:P5"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
     <mergeCell ref="O7:P7"/>
     <mergeCell ref="G1:K2"/>
     <mergeCell ref="B11:D11"/>
@@ -4799,59 +5101,28 @@
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="E6:F6"/>
-    <mergeCell ref="J4:P4"/>
-    <mergeCell ref="K5:P5"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="J14:O14"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B17:D17"/>
     <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="E17:F17"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B21:D21"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="J9:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4860,7 +5131,7 @@
   <dimension ref="B1:P1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="B16" sqref="B16:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4873,23 +5144,23 @@
   <sheetData>
     <row r="1" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G1" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
+        <v>33</v>
+      </c>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
     </row>
     <row r="2" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
     </row>
     <row r="3" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
@@ -4898,7 +5169,7 @@
       <c r="G3" s="20"/>
       <c r="H3" s="21"/>
       <c r="J3" s="19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K3" s="20"/>
       <c r="L3" s="20"/>
@@ -4909,10 +5180,10 @@
     </row>
     <row r="4" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>9</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
@@ -4920,10 +5191,10 @@
       <c r="G4" s="20"/>
       <c r="H4" s="21"/>
       <c r="J4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K4" s="23" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>9</v>
       </c>
       <c r="L4" s="20"/>
       <c r="M4" s="20"/>
@@ -4932,149 +5203,209 @@
       <c r="P4" s="21"/>
     </row>
     <row r="5" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="24" t="s">
-        <v>1</v>
+      <c r="B5" s="26" t="s">
+        <v>0</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="21"/>
       <c r="E5" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H5" s="21"/>
-      <c r="J5" s="24" t="s">
-        <v>1</v>
+      <c r="J5" s="26" t="s">
+        <v>0</v>
       </c>
       <c r="K5" s="20"/>
       <c r="L5" s="21"/>
       <c r="M5" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N5" s="21"/>
       <c r="O5" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P5" s="21"/>
     </row>
     <row r="6" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="23"/>
+      <c r="B6" s="24" t="s">
+        <v>3</v>
+      </c>
       <c r="C6" s="20"/>
       <c r="D6" s="21"/>
-      <c r="E6" s="23"/>
+      <c r="E6" s="24">
+        <v>2</v>
+      </c>
       <c r="F6" s="21"/>
-      <c r="G6" s="23"/>
+      <c r="G6" s="24">
+        <v>2</v>
+      </c>
       <c r="H6" s="21"/>
-      <c r="J6" s="23"/>
+      <c r="J6" s="24" t="s">
+        <v>39</v>
+      </c>
       <c r="K6" s="20"/>
       <c r="L6" s="21"/>
-      <c r="M6" s="23"/>
+      <c r="M6" s="24">
+        <v>1</v>
+      </c>
       <c r="N6" s="21"/>
-      <c r="O6" s="23"/>
+      <c r="O6" s="24">
+        <v>2</v>
+      </c>
       <c r="P6" s="21"/>
     </row>
     <row r="7" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="23"/>
+      <c r="B7" s="24" t="s">
+        <v>34</v>
+      </c>
       <c r="C7" s="20"/>
       <c r="D7" s="21"/>
-      <c r="E7" s="23"/>
+      <c r="E7" s="24">
+        <v>2</v>
+      </c>
       <c r="F7" s="21"/>
-      <c r="G7" s="23"/>
+      <c r="G7" s="24">
+        <v>3</v>
+      </c>
       <c r="H7" s="21"/>
-      <c r="J7" s="23"/>
+      <c r="J7" s="24" t="s">
+        <v>40</v>
+      </c>
       <c r="K7" s="20"/>
       <c r="L7" s="21"/>
-      <c r="M7" s="23"/>
+      <c r="M7" s="24">
+        <v>2</v>
+      </c>
       <c r="N7" s="21"/>
-      <c r="O7" s="23"/>
+      <c r="O7" s="24">
+        <v>2</v>
+      </c>
       <c r="P7" s="21"/>
     </row>
     <row r="8" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="23"/>
+      <c r="B8" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="C8" s="20"/>
       <c r="D8" s="21"/>
-      <c r="E8" s="19"/>
+      <c r="E8" s="24">
+        <v>1</v>
+      </c>
       <c r="F8" s="21"/>
-      <c r="G8" s="23"/>
+      <c r="G8" s="24">
+        <v>1</v>
+      </c>
       <c r="H8" s="21"/>
-      <c r="J8" s="23"/>
+      <c r="J8" s="24" t="s">
+        <v>41</v>
+      </c>
       <c r="K8" s="20"/>
       <c r="L8" s="21"/>
-      <c r="M8" s="19"/>
+      <c r="M8" s="24">
+        <v>1</v>
+      </c>
       <c r="N8" s="21"/>
-      <c r="O8" s="23"/>
+      <c r="O8" s="24">
+        <v>1</v>
+      </c>
       <c r="P8" s="21"/>
     </row>
     <row r="9" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="23"/>
+      <c r="B9" s="24" t="s">
+        <v>36</v>
+      </c>
       <c r="C9" s="20"/>
       <c r="D9" s="21"/>
-      <c r="E9" s="23"/>
+      <c r="E9" s="24" t="s">
+        <v>37</v>
+      </c>
       <c r="F9" s="21"/>
-      <c r="G9" s="23"/>
+      <c r="G9" s="24">
+        <v>1</v>
+      </c>
       <c r="H9" s="21"/>
-      <c r="J9" s="23"/>
+      <c r="J9" s="24" t="s">
+        <v>42</v>
+      </c>
       <c r="K9" s="20"/>
       <c r="L9" s="21"/>
-      <c r="M9" s="23"/>
+      <c r="M9" s="24" t="s">
+        <v>37</v>
+      </c>
       <c r="N9" s="21"/>
-      <c r="O9" s="23"/>
+      <c r="O9" s="24">
+        <v>1</v>
+      </c>
       <c r="P9" s="21"/>
     </row>
     <row r="10" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="23"/>
+      <c r="B10" s="24" t="s">
+        <v>47</v>
+      </c>
       <c r="C10" s="20"/>
       <c r="D10" s="21"/>
-      <c r="E10" s="23"/>
+      <c r="E10" s="24" t="s">
+        <v>37</v>
+      </c>
       <c r="F10" s="21"/>
-      <c r="G10" s="23"/>
+      <c r="G10" s="24">
+        <v>1</v>
+      </c>
       <c r="H10" s="21"/>
-      <c r="J10" s="23"/>
+      <c r="J10" s="24" t="s">
+        <v>48</v>
+      </c>
       <c r="K10" s="20"/>
       <c r="L10" s="21"/>
-      <c r="M10" s="23"/>
+      <c r="M10" s="24">
+        <v>2</v>
+      </c>
       <c r="N10" s="21"/>
-      <c r="O10" s="23"/>
+      <c r="O10" s="24">
+        <v>2</v>
+      </c>
       <c r="P10" s="21"/>
     </row>
     <row r="11" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="21"/>
       <c r="E11" s="19">
         <f>SUM(E6:F10)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="19">
         <f>SUM(G6:H10)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H11" s="21"/>
       <c r="J11" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K11" s="20"/>
       <c r="L11" s="21"/>
       <c r="M11" s="19">
         <f>SUM(M6:N10)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N11" s="21"/>
       <c r="O11" s="19">
         <f>SUM(O6:P10)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P11" s="21"/>
     </row>
     <row r="12" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
@@ -5083,7 +5414,7 @@
       <c r="G13" s="20"/>
       <c r="H13" s="21"/>
       <c r="J13" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
@@ -5093,10 +5424,10 @@
     </row>
     <row r="14" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>9</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
@@ -5105,54 +5436,70 @@
       <c r="H14" s="21"/>
       <c r="J14" s="4"/>
       <c r="K14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="M14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="N14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N14" s="2" t="s">
+      <c r="O14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O14" s="3" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="15" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="24" t="s">
-        <v>1</v>
+      <c r="B15" s="26" t="s">
+        <v>0</v>
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="21"/>
       <c r="E15" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H15" s="21"/>
       <c r="J15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="K15" s="4">
+        <v>15</v>
+      </c>
+      <c r="L15" s="4">
+        <v>7</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4">
+        <v>0</v>
+      </c>
+      <c r="O15" s="4">
+        <v>9</v>
+      </c>
     </row>
     <row r="16" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="23"/>
+      <c r="B16" s="24" t="s">
+        <v>49</v>
+      </c>
       <c r="C16" s="20"/>
       <c r="D16" s="21"/>
-      <c r="E16" s="23"/>
+      <c r="E16" s="24">
+        <v>3</v>
+      </c>
       <c r="F16" s="21"/>
-      <c r="G16" s="23"/>
+      <c r="G16" s="24">
+        <v>3</v>
+      </c>
       <c r="H16" s="21"/>
       <c r="J16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K16" s="4">
         <v>15</v>
@@ -5171,82 +5518,106 @@
       </c>
     </row>
     <row r="17" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="23"/>
+      <c r="B17" s="24" t="s">
+        <v>50</v>
+      </c>
       <c r="C17" s="20"/>
       <c r="D17" s="21"/>
-      <c r="E17" s="23"/>
+      <c r="E17" s="24">
+        <v>2</v>
+      </c>
       <c r="F17" s="21"/>
-      <c r="G17" s="23"/>
+      <c r="G17" s="24">
+        <v>2</v>
+      </c>
       <c r="H17" s="21"/>
     </row>
     <row r="18" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="23"/>
+      <c r="B18" s="24" t="s">
+        <v>41</v>
+      </c>
       <c r="C18" s="20"/>
       <c r="D18" s="21"/>
-      <c r="E18" s="23"/>
+      <c r="E18" s="24">
+        <v>1</v>
+      </c>
       <c r="F18" s="21"/>
-      <c r="G18" s="23"/>
+      <c r="G18" s="24">
+        <v>1</v>
+      </c>
       <c r="H18" s="21"/>
     </row>
     <row r="19" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="23"/>
+      <c r="B19" s="24" t="s">
+        <v>46</v>
+      </c>
       <c r="C19" s="20"/>
       <c r="D19" s="21"/>
-      <c r="E19" s="23"/>
+      <c r="E19" s="24" t="s">
+        <v>37</v>
+      </c>
       <c r="F19" s="21"/>
-      <c r="G19" s="23"/>
+      <c r="G19" s="24">
+        <v>1</v>
+      </c>
       <c r="H19" s="21"/>
     </row>
     <row r="20" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="23"/>
+      <c r="B20" s="24" t="s">
+        <v>51</v>
+      </c>
       <c r="C20" s="20"/>
       <c r="D20" s="21"/>
-      <c r="E20" s="23"/>
+      <c r="E20" s="24" t="s">
+        <v>37</v>
+      </c>
       <c r="F20" s="21"/>
-      <c r="G20" s="23"/>
+      <c r="G20" s="24">
+        <v>1</v>
+      </c>
       <c r="H20" s="21"/>
     </row>
     <row r="21" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="23"/>
+      <c r="B21" s="24"/>
       <c r="C21" s="20"/>
       <c r="D21" s="21"/>
-      <c r="E21" s="23"/>
+      <c r="E21" s="24"/>
       <c r="F21" s="21"/>
-      <c r="G21" s="23"/>
+      <c r="G21" s="24"/>
       <c r="H21" s="21"/>
     </row>
     <row r="22" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="23"/>
+      <c r="B22" s="24"/>
       <c r="C22" s="20"/>
       <c r="D22" s="21"/>
-      <c r="E22" s="23"/>
+      <c r="E22" s="24"/>
       <c r="F22" s="21"/>
-      <c r="G22" s="23"/>
+      <c r="G22" s="24"/>
       <c r="H22" s="21"/>
     </row>
     <row r="23" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="23"/>
+      <c r="B23" s="24"/>
       <c r="C23" s="20"/>
       <c r="D23" s="21"/>
-      <c r="E23" s="23"/>
+      <c r="E23" s="24"/>
       <c r="F23" s="21"/>
-      <c r="G23" s="23"/>
+      <c r="G23" s="24"/>
       <c r="H23" s="21"/>
     </row>
     <row r="24" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24" s="20"/>
       <c r="D24" s="21"/>
       <c r="E24" s="19">
         <f>SUM(E16:F23)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F24" s="21"/>
       <c r="G24" s="19">
         <f>SUM(G16:H23)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H24" s="21"/>
     </row>
@@ -6228,46 +6599,27 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J13:O13"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="G1:K2"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="J3:P3"/>
-    <mergeCell ref="K4:P4"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="E22:F22"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="G24:H24"/>
@@ -6281,33 +6633,52 @@
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="E22:F22"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="G19:H19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J13:O13"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="G1:K2"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="J3:P3"/>
+    <mergeCell ref="K4:P4"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -6320,7 +6691,7 @@
   <dimension ref="B1:P1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6332,23 +6703,23 @@
   <sheetData>
     <row r="1" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G1" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
+        <v>33</v>
+      </c>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
     </row>
     <row r="2" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
     </row>
     <row r="3" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
@@ -6357,7 +6728,7 @@
       <c r="G3" s="20"/>
       <c r="H3" s="21"/>
       <c r="J3" s="19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K3" s="20"/>
       <c r="L3" s="20"/>
@@ -6368,10 +6739,10 @@
     </row>
     <row r="4" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>24</v>
+        <v>7</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>23</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
@@ -6379,10 +6750,10 @@
       <c r="G4" s="20"/>
       <c r="H4" s="21"/>
       <c r="J4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K4" s="23" t="s">
-        <v>24</v>
+        <v>7</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>23</v>
       </c>
       <c r="L4" s="20"/>
       <c r="M4" s="20"/>
@@ -6391,149 +6762,197 @@
       <c r="P4" s="21"/>
     </row>
     <row r="5" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="24" t="s">
-        <v>1</v>
+      <c r="B5" s="26" t="s">
+        <v>0</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="21"/>
       <c r="E5" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H5" s="21"/>
-      <c r="J5" s="24" t="s">
-        <v>1</v>
+      <c r="J5" s="26" t="s">
+        <v>0</v>
       </c>
       <c r="K5" s="20"/>
       <c r="L5" s="21"/>
       <c r="M5" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N5" s="21"/>
       <c r="O5" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P5" s="21"/>
     </row>
     <row r="6" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="23"/>
+      <c r="B6" s="24" t="s">
+        <v>3</v>
+      </c>
       <c r="C6" s="20"/>
       <c r="D6" s="21"/>
-      <c r="E6" s="23"/>
+      <c r="E6" s="24">
+        <v>2</v>
+      </c>
       <c r="F6" s="21"/>
-      <c r="G6" s="23"/>
+      <c r="G6" s="24">
+        <v>2</v>
+      </c>
       <c r="H6" s="21"/>
-      <c r="J6" s="23"/>
+      <c r="J6" s="24" t="s">
+        <v>39</v>
+      </c>
       <c r="K6" s="20"/>
       <c r="L6" s="21"/>
-      <c r="M6" s="23"/>
+      <c r="M6" s="24">
+        <v>2</v>
+      </c>
       <c r="N6" s="21"/>
-      <c r="O6" s="23"/>
+      <c r="O6" s="24">
+        <v>2</v>
+      </c>
       <c r="P6" s="21"/>
     </row>
     <row r="7" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="23"/>
+      <c r="B7" s="24" t="s">
+        <v>34</v>
+      </c>
       <c r="C7" s="20"/>
       <c r="D7" s="21"/>
-      <c r="E7" s="23"/>
+      <c r="E7" s="24">
+        <v>2</v>
+      </c>
       <c r="F7" s="21"/>
-      <c r="G7" s="23"/>
+      <c r="G7" s="24">
+        <v>2</v>
+      </c>
       <c r="H7" s="21"/>
-      <c r="J7" s="23"/>
+      <c r="J7" s="24" t="s">
+        <v>40</v>
+      </c>
       <c r="K7" s="20"/>
       <c r="L7" s="21"/>
-      <c r="M7" s="23"/>
+      <c r="M7" s="24">
+        <v>3</v>
+      </c>
       <c r="N7" s="21"/>
-      <c r="O7" s="23"/>
+      <c r="O7" s="24">
+        <v>3</v>
+      </c>
       <c r="P7" s="21"/>
     </row>
     <row r="8" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="23"/>
+      <c r="B8" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="C8" s="20"/>
       <c r="D8" s="21"/>
-      <c r="E8" s="19"/>
+      <c r="E8" s="24">
+        <v>1</v>
+      </c>
       <c r="F8" s="21"/>
-      <c r="G8" s="23"/>
+      <c r="G8" s="24">
+        <v>1</v>
+      </c>
       <c r="H8" s="21"/>
-      <c r="J8" s="23"/>
+      <c r="J8" s="24" t="s">
+        <v>41</v>
+      </c>
       <c r="K8" s="20"/>
       <c r="L8" s="21"/>
-      <c r="M8" s="19"/>
+      <c r="M8" s="19">
+        <v>1</v>
+      </c>
       <c r="N8" s="21"/>
-      <c r="O8" s="23"/>
+      <c r="O8" s="24">
+        <v>1</v>
+      </c>
       <c r="P8" s="21"/>
     </row>
     <row r="9" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="23"/>
+      <c r="B9" s="24" t="s">
+        <v>36</v>
+      </c>
       <c r="C9" s="20"/>
       <c r="D9" s="21"/>
-      <c r="E9" s="23"/>
+      <c r="E9" s="24" t="s">
+        <v>37</v>
+      </c>
       <c r="F9" s="21"/>
-      <c r="G9" s="23"/>
+      <c r="G9" s="24">
+        <v>1</v>
+      </c>
       <c r="H9" s="21"/>
-      <c r="J9" s="23"/>
+      <c r="J9" s="24" t="s">
+        <v>42</v>
+      </c>
       <c r="K9" s="20"/>
       <c r="L9" s="21"/>
-      <c r="M9" s="23"/>
+      <c r="M9" s="24" t="s">
+        <v>37</v>
+      </c>
       <c r="N9" s="21"/>
-      <c r="O9" s="23"/>
+      <c r="O9" s="24">
+        <v>1</v>
+      </c>
       <c r="P9" s="21"/>
     </row>
     <row r="10" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="23"/>
+      <c r="B10" s="24"/>
       <c r="C10" s="20"/>
       <c r="D10" s="21"/>
-      <c r="E10" s="23"/>
+      <c r="E10" s="24"/>
       <c r="F10" s="21"/>
-      <c r="G10" s="23"/>
+      <c r="G10" s="24"/>
       <c r="H10" s="21"/>
-      <c r="J10" s="23"/>
+      <c r="J10" s="24"/>
       <c r="K10" s="20"/>
       <c r="L10" s="21"/>
-      <c r="M10" s="23"/>
+      <c r="M10" s="24"/>
       <c r="N10" s="21"/>
-      <c r="O10" s="23"/>
+      <c r="O10" s="24"/>
       <c r="P10" s="21"/>
     </row>
     <row r="11" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="21"/>
       <c r="E11" s="19">
         <f>SUM(E6:F10)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="19">
         <f>SUM(G6:H10)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H11" s="21"/>
       <c r="J11" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K11" s="20"/>
       <c r="L11" s="21"/>
       <c r="M11" s="19">
         <f>SUM(M6:N10)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N11" s="21"/>
       <c r="O11" s="19">
         <f>SUM(O6:P10)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="P11" s="21"/>
     </row>
     <row r="12" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
@@ -6542,7 +6961,7 @@
       <c r="G13" s="20"/>
       <c r="H13" s="21"/>
       <c r="J13" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
@@ -6552,10 +6971,10 @@
     </row>
     <row r="14" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>24</v>
+        <v>7</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>23</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
@@ -6564,54 +6983,70 @@
       <c r="H14" s="21"/>
       <c r="J14" s="4"/>
       <c r="K14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="M14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="N14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N14" s="2" t="s">
+      <c r="O14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O14" s="3" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="15" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="24" t="s">
-        <v>1</v>
+      <c r="B15" s="26" t="s">
+        <v>0</v>
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="21"/>
       <c r="E15" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H15" s="21"/>
       <c r="J15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="K15" s="4">
+        <v>15</v>
+      </c>
+      <c r="L15" s="4">
+        <v>9</v>
+      </c>
+      <c r="M15" s="4">
+        <v>2</v>
+      </c>
+      <c r="N15" s="4">
+        <v>0</v>
+      </c>
+      <c r="O15" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="23"/>
+      <c r="B16" s="24" t="s">
+        <v>43</v>
+      </c>
       <c r="C16" s="20"/>
       <c r="D16" s="21"/>
-      <c r="E16" s="23"/>
+      <c r="E16" s="24">
+        <v>2</v>
+      </c>
       <c r="F16" s="21"/>
-      <c r="G16" s="23"/>
+      <c r="G16" s="24">
+        <v>2</v>
+      </c>
       <c r="H16" s="21"/>
       <c r="J16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K16" s="4">
         <v>15</v>
@@ -6630,82 +7065,106 @@
       </c>
     </row>
     <row r="17" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="23"/>
+      <c r="B17" s="24" t="s">
+        <v>52</v>
+      </c>
       <c r="C17" s="20"/>
       <c r="D17" s="21"/>
-      <c r="E17" s="23"/>
+      <c r="E17" s="24">
+        <v>2</v>
+      </c>
       <c r="F17" s="21"/>
-      <c r="G17" s="23"/>
+      <c r="G17" s="24">
+        <v>2</v>
+      </c>
       <c r="H17" s="21"/>
     </row>
     <row r="18" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="23"/>
+      <c r="B18" s="24" t="s">
+        <v>41</v>
+      </c>
       <c r="C18" s="20"/>
       <c r="D18" s="21"/>
-      <c r="E18" s="23"/>
+      <c r="E18" s="24">
+        <v>1</v>
+      </c>
       <c r="F18" s="21"/>
-      <c r="G18" s="23"/>
+      <c r="G18" s="24">
+        <v>1</v>
+      </c>
       <c r="H18" s="21"/>
     </row>
     <row r="19" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="23"/>
+      <c r="B19" s="24" t="s">
+        <v>46</v>
+      </c>
       <c r="C19" s="20"/>
       <c r="D19" s="21"/>
-      <c r="E19" s="23"/>
+      <c r="E19" s="24" t="s">
+        <v>37</v>
+      </c>
       <c r="F19" s="21"/>
-      <c r="G19" s="23"/>
+      <c r="G19" s="24">
+        <v>1</v>
+      </c>
       <c r="H19" s="21"/>
     </row>
     <row r="20" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="23"/>
+      <c r="B20" s="24" t="s">
+        <v>51</v>
+      </c>
       <c r="C20" s="20"/>
       <c r="D20" s="21"/>
-      <c r="E20" s="23"/>
+      <c r="E20" s="24">
+        <v>1</v>
+      </c>
       <c r="F20" s="21"/>
-      <c r="G20" s="23"/>
+      <c r="G20" s="24">
+        <v>1</v>
+      </c>
       <c r="H20" s="21"/>
     </row>
     <row r="21" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="23"/>
+      <c r="B21" s="24"/>
       <c r="C21" s="20"/>
       <c r="D21" s="21"/>
-      <c r="E21" s="23"/>
+      <c r="E21" s="24"/>
       <c r="F21" s="21"/>
-      <c r="G21" s="23"/>
+      <c r="G21" s="24"/>
       <c r="H21" s="21"/>
     </row>
     <row r="22" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="23"/>
+      <c r="B22" s="24"/>
       <c r="C22" s="20"/>
       <c r="D22" s="21"/>
-      <c r="E22" s="23"/>
+      <c r="E22" s="24"/>
       <c r="F22" s="21"/>
-      <c r="G22" s="23"/>
+      <c r="G22" s="24"/>
       <c r="H22" s="21"/>
     </row>
     <row r="23" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="23"/>
+      <c r="B23" s="24"/>
       <c r="C23" s="20"/>
       <c r="D23" s="21"/>
-      <c r="E23" s="23"/>
+      <c r="E23" s="24"/>
       <c r="F23" s="21"/>
-      <c r="G23" s="23"/>
+      <c r="G23" s="24"/>
       <c r="H23" s="21"/>
     </row>
     <row r="24" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24" s="20"/>
       <c r="D24" s="21"/>
       <c r="E24" s="19">
         <f>SUM(E16:F23)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F24" s="21"/>
       <c r="G24" s="19">
         <f>SUM(G16:H23)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H24" s="21"/>
     </row>
@@ -7687,46 +8146,27 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J13:O13"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="G1:K2"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="J3:P3"/>
-    <mergeCell ref="K4:P4"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="E22:F22"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="G24:H24"/>
@@ -7740,33 +8180,52 @@
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="E22:F22"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="G19:H19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J13:O13"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="G1:K2"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="J3:P3"/>
+    <mergeCell ref="K4:P4"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -7779,7 +8238,7 @@
   <dimension ref="B1:P1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17:H18"/>
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7791,23 +8250,23 @@
   <sheetData>
     <row r="1" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G1" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
+        <v>33</v>
+      </c>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
     </row>
     <row r="2" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
     </row>
     <row r="3" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
@@ -7816,7 +8275,7 @@
       <c r="G3" s="20"/>
       <c r="H3" s="21"/>
       <c r="J3" s="19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K3" s="20"/>
       <c r="L3" s="20"/>
@@ -7827,10 +8286,10 @@
     </row>
     <row r="4" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>26</v>
+        <v>7</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>25</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
@@ -7838,10 +8297,10 @@
       <c r="G4" s="20"/>
       <c r="H4" s="21"/>
       <c r="J4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K4" s="23" t="s">
-        <v>26</v>
+        <v>7</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>25</v>
       </c>
       <c r="L4" s="20"/>
       <c r="M4" s="20"/>
@@ -7850,149 +8309,209 @@
       <c r="P4" s="21"/>
     </row>
     <row r="5" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="24" t="s">
-        <v>1</v>
+      <c r="B5" s="26" t="s">
+        <v>0</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="21"/>
       <c r="E5" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H5" s="21"/>
-      <c r="J5" s="24" t="s">
-        <v>1</v>
+      <c r="J5" s="26" t="s">
+        <v>0</v>
       </c>
       <c r="K5" s="20"/>
       <c r="L5" s="21"/>
       <c r="M5" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N5" s="21"/>
       <c r="O5" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P5" s="21"/>
     </row>
     <row r="6" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="23"/>
+      <c r="B6" s="24" t="s">
+        <v>3</v>
+      </c>
       <c r="C6" s="20"/>
       <c r="D6" s="21"/>
-      <c r="E6" s="23"/>
+      <c r="E6" s="24">
+        <v>2</v>
+      </c>
       <c r="F6" s="21"/>
-      <c r="G6" s="23"/>
+      <c r="G6" s="24">
+        <v>2</v>
+      </c>
       <c r="H6" s="21"/>
-      <c r="J6" s="23"/>
+      <c r="J6" s="24" t="s">
+        <v>39</v>
+      </c>
       <c r="K6" s="20"/>
       <c r="L6" s="21"/>
-      <c r="M6" s="23"/>
+      <c r="M6" s="24">
+        <v>2</v>
+      </c>
       <c r="N6" s="21"/>
-      <c r="O6" s="23"/>
+      <c r="O6" s="24">
+        <v>2</v>
+      </c>
       <c r="P6" s="21"/>
     </row>
     <row r="7" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="23"/>
+      <c r="B7" s="24" t="s">
+        <v>34</v>
+      </c>
       <c r="C7" s="20"/>
       <c r="D7" s="21"/>
-      <c r="E7" s="23"/>
+      <c r="E7" s="24">
+        <v>2</v>
+      </c>
       <c r="F7" s="21"/>
-      <c r="G7" s="23"/>
+      <c r="G7" s="24">
+        <v>2</v>
+      </c>
       <c r="H7" s="21"/>
-      <c r="J7" s="23"/>
+      <c r="J7" s="24" t="s">
+        <v>40</v>
+      </c>
       <c r="K7" s="20"/>
       <c r="L7" s="21"/>
-      <c r="M7" s="23"/>
+      <c r="M7" s="24">
+        <v>3</v>
+      </c>
       <c r="N7" s="21"/>
-      <c r="O7" s="23"/>
+      <c r="O7" s="24">
+        <v>3</v>
+      </c>
       <c r="P7" s="21"/>
     </row>
     <row r="8" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="23"/>
+      <c r="B8" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="C8" s="20"/>
       <c r="D8" s="21"/>
-      <c r="E8" s="19"/>
+      <c r="E8" s="24">
+        <v>1</v>
+      </c>
       <c r="F8" s="21"/>
-      <c r="G8" s="23"/>
+      <c r="G8" s="24">
+        <v>1</v>
+      </c>
       <c r="H8" s="21"/>
-      <c r="J8" s="23"/>
+      <c r="J8" s="24" t="s">
+        <v>41</v>
+      </c>
       <c r="K8" s="20"/>
       <c r="L8" s="21"/>
-      <c r="M8" s="19"/>
+      <c r="M8" s="19">
+        <v>1</v>
+      </c>
       <c r="N8" s="21"/>
-      <c r="O8" s="23"/>
+      <c r="O8" s="24">
+        <v>1</v>
+      </c>
       <c r="P8" s="21"/>
     </row>
     <row r="9" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="23"/>
+      <c r="B9" s="24" t="s">
+        <v>36</v>
+      </c>
       <c r="C9" s="20"/>
       <c r="D9" s="21"/>
-      <c r="E9" s="23"/>
+      <c r="E9" s="24" t="s">
+        <v>37</v>
+      </c>
       <c r="F9" s="21"/>
-      <c r="G9" s="23"/>
+      <c r="G9" s="24">
+        <v>1</v>
+      </c>
       <c r="H9" s="21"/>
-      <c r="J9" s="23"/>
+      <c r="J9" s="24" t="s">
+        <v>42</v>
+      </c>
       <c r="K9" s="20"/>
       <c r="L9" s="21"/>
-      <c r="M9" s="23"/>
+      <c r="M9" s="24" t="s">
+        <v>37</v>
+      </c>
       <c r="N9" s="21"/>
-      <c r="O9" s="23"/>
+      <c r="O9" s="24">
+        <v>1</v>
+      </c>
       <c r="P9" s="21"/>
     </row>
     <row r="10" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="23"/>
+      <c r="B10" s="24" t="s">
+        <v>47</v>
+      </c>
       <c r="C10" s="20"/>
       <c r="D10" s="21"/>
-      <c r="E10" s="23"/>
+      <c r="E10" s="24" t="s">
+        <v>37</v>
+      </c>
       <c r="F10" s="21"/>
-      <c r="G10" s="23"/>
+      <c r="G10" s="24">
+        <v>1</v>
+      </c>
       <c r="H10" s="21"/>
-      <c r="J10" s="23"/>
+      <c r="J10" s="24" t="s">
+        <v>53</v>
+      </c>
       <c r="K10" s="20"/>
       <c r="L10" s="21"/>
-      <c r="M10" s="23"/>
+      <c r="M10" s="24">
+        <v>2</v>
+      </c>
       <c r="N10" s="21"/>
-      <c r="O10" s="23"/>
+      <c r="O10" s="24">
+        <v>3</v>
+      </c>
       <c r="P10" s="21"/>
     </row>
     <row r="11" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="21"/>
       <c r="E11" s="19">
         <f>SUM(E6:F10)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="19">
         <f>SUM(G6:H10)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H11" s="21"/>
       <c r="J11" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K11" s="20"/>
       <c r="L11" s="21"/>
       <c r="M11" s="19">
         <f>SUM(M6:N10)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N11" s="21"/>
       <c r="O11" s="19">
         <f>SUM(O6:P10)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P11" s="21"/>
     </row>
     <row r="12" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
@@ -8001,7 +8520,7 @@
       <c r="G13" s="20"/>
       <c r="H13" s="21"/>
       <c r="J13" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
@@ -8011,10 +8530,10 @@
     </row>
     <row r="14" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>26</v>
+        <v>7</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>25</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
@@ -8023,54 +8542,70 @@
       <c r="H14" s="21"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="M14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="N14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N14" s="2" t="s">
+      <c r="O14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O14" s="3" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="15" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="24" t="s">
-        <v>1</v>
+      <c r="B15" s="26" t="s">
+        <v>0</v>
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="21"/>
       <c r="E15" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H15" s="21"/>
       <c r="J15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="K15" s="4">
+        <v>15</v>
+      </c>
+      <c r="L15" s="4">
+        <v>8</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4">
+        <v>0</v>
+      </c>
+      <c r="O15" s="4">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="23"/>
+      <c r="B16" s="24" t="s">
+        <v>54</v>
+      </c>
       <c r="C16" s="20"/>
       <c r="D16" s="21"/>
-      <c r="E16" s="23"/>
+      <c r="E16" s="24">
+        <v>2</v>
+      </c>
       <c r="F16" s="21"/>
-      <c r="G16" s="23"/>
+      <c r="G16" s="24">
+        <v>3</v>
+      </c>
       <c r="H16" s="21"/>
       <c r="J16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K16" s="4">
         <v>15</v>
@@ -8089,83 +8624,107 @@
       </c>
     </row>
     <row r="17" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="23"/>
+      <c r="B17" s="24" t="s">
+        <v>50</v>
+      </c>
       <c r="C17" s="20"/>
       <c r="D17" s="21"/>
-      <c r="E17" s="23"/>
+      <c r="E17" s="24">
+        <v>2</v>
+      </c>
       <c r="F17" s="21"/>
-      <c r="G17" s="23"/>
+      <c r="G17" s="24">
+        <v>2</v>
+      </c>
       <c r="H17" s="21"/>
       <c r="J17" s="7"/>
     </row>
     <row r="18" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="23"/>
+      <c r="B18" s="24" t="s">
+        <v>41</v>
+      </c>
       <c r="C18" s="20"/>
       <c r="D18" s="21"/>
-      <c r="E18" s="23"/>
+      <c r="E18" s="24">
+        <v>1</v>
+      </c>
       <c r="F18" s="21"/>
-      <c r="G18" s="23"/>
+      <c r="G18" s="24">
+        <v>1</v>
+      </c>
       <c r="H18" s="21"/>
     </row>
     <row r="19" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="23"/>
+      <c r="B19" s="24" t="s">
+        <v>46</v>
+      </c>
       <c r="C19" s="20"/>
       <c r="D19" s="21"/>
-      <c r="E19" s="23"/>
+      <c r="E19" s="24" t="s">
+        <v>37</v>
+      </c>
       <c r="F19" s="21"/>
-      <c r="G19" s="23"/>
+      <c r="G19" s="24">
+        <v>1</v>
+      </c>
       <c r="H19" s="21"/>
     </row>
     <row r="20" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="23"/>
+      <c r="B20" s="24" t="s">
+        <v>51</v>
+      </c>
       <c r="C20" s="20"/>
       <c r="D20" s="21"/>
-      <c r="E20" s="23"/>
+      <c r="E20" s="24">
+        <v>1</v>
+      </c>
       <c r="F20" s="21"/>
-      <c r="G20" s="23"/>
+      <c r="G20" s="24">
+        <v>1</v>
+      </c>
       <c r="H20" s="21"/>
     </row>
     <row r="21" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="23"/>
+      <c r="B21" s="24"/>
       <c r="C21" s="20"/>
       <c r="D21" s="21"/>
-      <c r="E21" s="23"/>
+      <c r="E21" s="24"/>
       <c r="F21" s="21"/>
-      <c r="G21" s="23"/>
+      <c r="G21" s="24"/>
       <c r="H21" s="21"/>
     </row>
     <row r="22" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="23"/>
+      <c r="B22" s="24"/>
       <c r="C22" s="20"/>
       <c r="D22" s="21"/>
-      <c r="E22" s="23"/>
+      <c r="E22" s="24"/>
       <c r="F22" s="21"/>
-      <c r="G22" s="23"/>
+      <c r="G22" s="24"/>
       <c r="H22" s="21"/>
     </row>
     <row r="23" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="23"/>
+      <c r="B23" s="24"/>
       <c r="C23" s="20"/>
       <c r="D23" s="21"/>
-      <c r="E23" s="23"/>
+      <c r="E23" s="24"/>
       <c r="F23" s="21"/>
-      <c r="G23" s="23"/>
+      <c r="G23" s="24"/>
       <c r="H23" s="21"/>
     </row>
     <row r="24" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24" s="20"/>
       <c r="D24" s="21"/>
       <c r="E24" s="19">
         <f>SUM(E16:F23)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F24" s="21"/>
       <c r="G24" s="19">
         <f>SUM(G16:H23)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H24" s="21"/>
     </row>
@@ -9147,46 +9706,27 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J13:O13"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="G1:K2"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="J3:P3"/>
-    <mergeCell ref="K4:P4"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="E22:F22"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="G24:H24"/>
@@ -9200,33 +9740,52 @@
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="E22:F22"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="G19:H19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J13:O13"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="G1:K2"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="J3:P3"/>
+    <mergeCell ref="K4:P4"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -9239,7 +9798,7 @@
   <dimension ref="B1:O1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P16" sqref="P16:P17"/>
+      <selection activeCell="M13" sqref="M12:M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9254,39 +9813,39 @@
   <sheetData>
     <row r="1" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F1" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
+        <v>33</v>
+      </c>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
     </row>
     <row r="2" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
     </row>
     <row r="3" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
       <c r="E4" s="21"/>
       <c r="F4" s="5"/>
       <c r="G4" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
       <c r="J4" s="21"/>
-      <c r="L4" s="26" t="s">
-        <v>28</v>
+      <c r="L4" s="27" t="s">
+        <v>27</v>
       </c>
       <c r="M4" s="20"/>
       <c r="N4" s="20"/>
@@ -9294,101 +9853,107 @@
     </row>
     <row r="5" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="21"/>
       <c r="D5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H5" s="21"/>
       <c r="I5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L5" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M5" s="21"/>
       <c r="N5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="23" t="s">
-        <v>36</v>
+      <c r="B6" s="24" t="s">
+        <v>33</v>
       </c>
       <c r="C6" s="21"/>
       <c r="D6" s="4">
         <v>20</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="4">
+        <v>29</v>
+      </c>
       <c r="F6" s="5"/>
-      <c r="G6" s="23" t="s">
-        <v>36</v>
+      <c r="G6" s="24" t="s">
+        <v>33</v>
       </c>
       <c r="H6" s="21"/>
       <c r="I6" s="4">
         <v>20</v>
       </c>
-      <c r="J6" s="4"/>
-      <c r="L6" s="23" t="s">
-        <v>36</v>
+      <c r="J6" s="4">
+        <v>32</v>
+      </c>
+      <c r="L6" s="24" t="s">
+        <v>33</v>
       </c>
       <c r="M6" s="21"/>
       <c r="N6" s="4">
         <v>20</v>
       </c>
-      <c r="O6" s="4"/>
+      <c r="O6" s="4">
+        <v>32</v>
+      </c>
     </row>
     <row r="7" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="21"/>
       <c r="D7" s="4">
         <v>20</v>
       </c>
       <c r="E7" s="4">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H7" s="21"/>
       <c r="I7" s="4">
         <v>20</v>
       </c>
       <c r="J7" s="4">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="L7" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M7" s="21"/>
       <c r="N7" s="4">
         <v>20</v>
       </c>
       <c r="O7" s="6">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
@@ -9396,7 +9961,7 @@
       <c r="F9" s="21"/>
       <c r="H9" s="5"/>
       <c r="I9" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="21"/>
@@ -9404,20 +9969,20 @@
     <row r="10" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
       <c r="C10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J10" s="21"/>
       <c r="K10" s="4">
@@ -9427,24 +9992,34 @@
     </row>
     <row r="11" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="C11" s="4">
+        <v>60</v>
+      </c>
+      <c r="D11" s="4">
+        <f>C11-E7</f>
+        <v>31</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
       <c r="F11" s="4">
         <v>0</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J11" s="21"/>
-      <c r="K11" s="4"/>
+      <c r="K11" s="4">
+        <f>E7+J7+O7</f>
+        <v>93</v>
+      </c>
     </row>
     <row r="12" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="4">
         <v>60</v>
@@ -9460,10 +10035,13 @@
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J12" s="21"/>
-      <c r="K12" s="4"/>
+      <c r="K12" s="4">
+        <f>K11-K10</f>
+        <v>33</v>
+      </c>
     </row>
     <row r="13" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10455,12 +11033,6 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B9:F9"/>
     <mergeCell ref="L7:M7"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="G6:H6"/>
@@ -10473,6 +11045,12 @@
     <mergeCell ref="L4:O4"/>
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="L6:M6"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>